<commit_message>
This is the second Test code
</commit_message>
<xml_diff>
--- a/Salary_Data.csv.xlsx
+++ b/Salary_Data.csv.xlsx
@@ -361,7 +361,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -623,6 +625,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B3:B32">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>